<commit_message>
funcion para agreagar las obs de las estaciones
</commit_message>
<xml_diff>
--- a/info_wunder.xlsx
+++ b/info_wunder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\tecnicatura_ia\adscripcion\wunder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AF4174-C2A6-42DA-A7C1-E2B778AD3AB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEDBF2B-C2B9-4E6D-B83A-0097A584A5DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,6 +1110,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1128,10 +1132,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1139,10 +1139,10 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
@@ -1246,23 +1246,17 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F1D090AC-1028-4E37-8AF3-21AF76AA1915}" name="Table3" displayName="Table3" ref="A1:F144" totalsRowShown="0">
-  <autoFilter ref="A1:F144" xr:uid="{0178986E-7A41-44C1-BFAB-9C4133D6CE5D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="IROSAR5"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F144" xr:uid="{0178986E-7A41-44C1-BFAB-9C4133D6CE5D}"/>
   <sortState ref="A2:F144">
-    <sortCondition ref="B1:B144"/>
+    <sortCondition ref="C1:C144"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{32E268D2-049C-4DC8-A1E2-52ADDED4FC74}" name="índice" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D40DACC-075A-47A6-8206-96627E160B72}" name="id" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{5AF1C093-77D3-4351-81A5-6EEB9E2ADA96}" name="inicio" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{81953E3E-C968-4444-9FE5-4633B7C51C99}" name="fecha_ultimo_reporte" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{AB0A46F0-AC6A-4779-ADBF-1D9936A32704}" name="dias_obs" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{D21B3D98-A9FF-42E6-8F6A-AA58B6B9CACD}" name="buscar_obs" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{AB0A46F0-AC6A-4779-ADBF-1D9936A32704}" name="dias_obs" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{D21B3D98-A9FF-42E6-8F6A-AA58B6B9CACD}" name="buscar_obs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1476,7 +1470,7 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,22 +1505,22 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="13.35" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
+        <v>131</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="C2" s="22">
-        <v>44874</v>
+        <v>41049</v>
       </c>
       <c r="D2" s="4">
         <v>45546</v>
       </c>
-      <c r="E2" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>672</v>
+      <c r="E2" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>4497</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1535,22 +1529,22 @@
       <c r="I2"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="13.35" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C3" s="22">
-        <v>44986</v>
+        <v>41350</v>
       </c>
       <c r="D3" s="4">
         <v>45546</v>
       </c>
-      <c r="E3" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>560</v>
+      <c r="E3" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>4196</v>
       </c>
       <c r="F3" s="21">
         <v>0</v>
@@ -1560,22 +1554,22 @@
       <c r="I3"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="13.35" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>132</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="C4" s="22">
-        <v>45067</v>
-      </c>
-      <c r="D4" s="32">
-        <v>45344.902569444443</v>
-      </c>
-      <c r="E4" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>277.90256944444263</v>
+        <v>41674</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E4" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>3872</v>
       </c>
       <c r="F4" s="21">
         <v>0</v>
@@ -1585,22 +1579,22 @@
       <c r="I4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="22">
-        <v>45040</v>
-      </c>
-      <c r="D5" s="32">
-        <v>45407.999849537038</v>
-      </c>
-      <c r="E5" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>367.99984953703824</v>
+        <v>42208</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E5" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>3338</v>
       </c>
       <c r="F5" s="21">
         <v>0</v>
@@ -1609,22 +1603,22 @@
       <c r="H5" s="34"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>9</v>
+        <v>133</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="C6" s="22">
-        <v>44172</v>
+        <v>42403</v>
       </c>
       <c r="D6" s="4">
         <v>45546</v>
       </c>
-      <c r="E6" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1374</v>
+      <c r="E6" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>3143</v>
       </c>
       <c r="F6" s="21">
         <v>0</v>
@@ -1634,22 +1628,22 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C7" s="22">
-        <v>44943</v>
+        <v>42736</v>
       </c>
       <c r="D7" s="4">
         <v>45546</v>
       </c>
-      <c r="E7" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>603</v>
+      <c r="E7" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2810</v>
       </c>
       <c r="F7" s="21">
         <v>0</v>
@@ -1658,22 +1652,22 @@
       <c r="H7" s="34"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="C8" s="22">
-        <v>45124</v>
+        <v>42736</v>
       </c>
       <c r="D8" s="4">
         <v>45546</v>
       </c>
-      <c r="E8" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>422</v>
+      <c r="E8" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2810</v>
       </c>
       <c r="F8" s="21">
         <v>0</v>
@@ -1682,22 +1676,22 @@
       <c r="H8" s="34"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C9" s="22">
-        <v>45104</v>
+        <v>42826</v>
       </c>
       <c r="D9" s="4">
         <v>45546</v>
       </c>
-      <c r="E9" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>442</v>
+      <c r="E9" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2720</v>
       </c>
       <c r="F9" s="21">
         <v>0</v>
@@ -1706,22 +1700,22 @@
       <c r="H9" s="34"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C10" s="22">
-        <v>45136</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E10" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>410</v>
+        <v>42833</v>
+      </c>
+      <c r="D10" s="32">
+        <v>45360.991597222222</v>
+      </c>
+      <c r="E10" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2527.9915972222225</v>
       </c>
       <c r="F10" s="21">
         <v>0</v>
@@ -1730,22 +1724,22 @@
       <c r="H10" s="34"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>10</v>
+        <v>126</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C11" s="22">
-        <v>44106</v>
+        <v>42866</v>
       </c>
       <c r="D11" s="4">
         <v>45546</v>
       </c>
-      <c r="E11" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1440</v>
+      <c r="E11" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2680</v>
       </c>
       <c r="F11" s="21">
         <v>0</v>
@@ -1754,22 +1748,22 @@
       <c r="H11" s="34"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="C12" s="22">
-        <v>44461</v>
+        <v>42940</v>
       </c>
       <c r="D12" s="4">
         <v>45546</v>
       </c>
-      <c r="E12" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1085</v>
+      <c r="E12" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2606</v>
       </c>
       <c r="F12" s="21">
         <v>0</v>
@@ -1778,22 +1772,22 @@
       <c r="H12" s="34"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C13" s="22">
-        <v>43827</v>
+        <v>43163</v>
       </c>
       <c r="D13" s="4">
         <v>45546</v>
       </c>
-      <c r="E13" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1719</v>
+      <c r="E13" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2383</v>
       </c>
       <c r="F13" s="21">
         <v>0</v>
@@ -1803,22 +1797,22 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C14" s="22">
-        <v>44040</v>
+        <v>43245</v>
       </c>
       <c r="D14" s="4">
         <v>45546</v>
       </c>
-      <c r="E14" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1506</v>
+      <c r="E14" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2301</v>
       </c>
       <c r="F14" s="21">
         <v>0</v>
@@ -1827,22 +1821,22 @@
       <c r="H14" s="34"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C15" s="22">
-        <v>44194</v>
+        <v>43329</v>
       </c>
       <c r="D15" s="4">
         <v>45546</v>
       </c>
-      <c r="E15" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1352</v>
+      <c r="E15" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2217</v>
       </c>
       <c r="F15" s="21">
         <v>0</v>
@@ -1851,22 +1845,22 @@
       <c r="H15" s="34"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="C16" s="22">
-        <v>44358</v>
+        <v>43349</v>
       </c>
       <c r="D16" s="4">
         <v>45546</v>
       </c>
-      <c r="E16" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1188</v>
+      <c r="E16" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2197</v>
       </c>
       <c r="F16" s="21">
         <v>0</v>
@@ -1875,22 +1869,22 @@
       <c r="H16" s="34"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="C17" s="22">
-        <v>44534</v>
+        <v>43357</v>
       </c>
       <c r="D17" s="4">
         <v>45546</v>
       </c>
-      <c r="E17" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1012</v>
+      <c r="E17" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2189</v>
       </c>
       <c r="F17" s="21">
         <v>0</v>
@@ -1899,22 +1893,22 @@
       <c r="H17" s="34"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="C18" s="22">
-        <v>44738</v>
+        <v>43419</v>
       </c>
       <c r="D18" s="4">
         <v>45546</v>
       </c>
-      <c r="E18" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>808</v>
+      <c r="E18" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2127</v>
       </c>
       <c r="F18" s="14">
         <v>0</v>
@@ -1922,22 +1916,22 @@
       <c r="G18" s="2"/>
       <c r="H18" s="34"/>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C19" s="22">
-        <v>44819</v>
+        <v>43433</v>
       </c>
       <c r="D19" s="4">
         <v>45546</v>
       </c>
-      <c r="E19" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>727</v>
+      <c r="E19" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2113</v>
       </c>
       <c r="F19" s="14">
         <v>0</v>
@@ -1946,20 +1940,23 @@
       <c r="H19" s="34"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="D20" t="s">
-        <v>264</v>
-      </c>
-      <c r="E20" s="42"/>
+        <v>119</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43487</v>
+      </c>
+      <c r="D20" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E20" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2059</v>
+      </c>
       <c r="F20" s="21">
         <v>0</v>
       </c>
@@ -1967,22 +1964,22 @@
       <c r="H20" s="34"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C21" s="22">
-        <v>44923</v>
+        <v>43535</v>
       </c>
       <c r="D21" s="4">
         <v>45546</v>
       </c>
-      <c r="E21" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>623</v>
+      <c r="E21" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>2011</v>
       </c>
       <c r="F21" s="21">
         <v>0</v>
@@ -1991,22 +1988,22 @@
       <c r="H21" s="34"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C22" s="22">
-        <v>42736</v>
+        <v>43568</v>
       </c>
       <c r="D22" s="4">
         <v>45546</v>
       </c>
-      <c r="E22" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2810</v>
+      <c r="E22" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1978</v>
       </c>
       <c r="F22" s="24">
         <v>0</v>
@@ -2015,22 +2012,22 @@
       <c r="H22" s="34"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>23</v>
+        <v>137</v>
       </c>
       <c r="C23" s="22">
-        <v>44680</v>
-      </c>
-      <c r="D23" s="32">
-        <v>45525.999895833331</v>
-      </c>
-      <c r="E23" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>845.99989583333081</v>
+        <v>43572</v>
+      </c>
+      <c r="D23" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E23" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1974</v>
       </c>
       <c r="F23" s="24">
         <v>0</v>
@@ -2039,22 +2036,22 @@
       <c r="H23" s="34"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="C24" s="22">
-        <v>42826</v>
+        <v>43612</v>
       </c>
       <c r="D24" s="4">
         <v>45546</v>
       </c>
-      <c r="E24" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2720</v>
+      <c r="E24" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1934</v>
       </c>
       <c r="F24" s="24">
         <v>0</v>
@@ -2063,22 +2060,22 @@
       <c r="H24" s="34"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="C25" s="22">
-        <v>42833</v>
-      </c>
-      <c r="D25" s="32">
-        <v>45360.991597222222</v>
-      </c>
-      <c r="E25" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2527.9915972222225</v>
+        <v>43621</v>
+      </c>
+      <c r="D25" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E25" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1925</v>
       </c>
       <c r="F25" s="24">
         <v>0</v>
@@ -2087,22 +2084,22 @@
       <c r="H25" s="34"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="C26" s="22">
-        <v>43163</v>
-      </c>
-      <c r="D26" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E26" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2383</v>
+        <v>43650</v>
+      </c>
+      <c r="D26" s="32">
+        <v>45542.998993055553</v>
+      </c>
+      <c r="E26" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1892.998993055553</v>
       </c>
       <c r="F26" s="24">
         <v>0</v>
@@ -2111,22 +2108,22 @@
       <c r="H26" s="34"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C27" s="22">
-        <v>41350</v>
+        <v>43729</v>
       </c>
       <c r="D27" s="4">
         <v>45546</v>
       </c>
-      <c r="E27" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>4196</v>
+      <c r="E27" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1817</v>
       </c>
       <c r="F27" s="24">
         <v>0</v>
@@ -2135,22 +2132,22 @@
       <c r="H27" s="34"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C28" s="22">
-        <v>42208</v>
+        <v>43736</v>
       </c>
       <c r="D28" s="4">
         <v>45546</v>
       </c>
-      <c r="E28" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>3338</v>
+      <c r="E28" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1810</v>
       </c>
       <c r="F28" s="24">
         <v>0</v>
@@ -2159,22 +2156,22 @@
       <c r="H28" s="34"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C29" s="22">
-        <v>44282</v>
+        <v>43799</v>
       </c>
       <c r="D29" s="4">
         <v>45546</v>
       </c>
-      <c r="E29" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1264</v>
+      <c r="E29" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1747</v>
       </c>
       <c r="F29" s="24">
         <v>0</v>
@@ -2183,22 +2180,22 @@
       <c r="H29" s="34"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C30" s="22">
-        <v>44418</v>
-      </c>
-      <c r="D30" s="32">
-        <v>45468.999965277777</v>
-      </c>
-      <c r="E30" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1050.9999652777769</v>
+        <v>43827</v>
+      </c>
+      <c r="D30" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E30" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1719</v>
       </c>
       <c r="F30" s="24">
         <v>0</v>
@@ -2207,22 +2204,22 @@
       <c r="H30" s="34"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="C31" s="22">
-        <v>44866</v>
+        <v>43864</v>
       </c>
       <c r="D31" s="4">
         <v>45546</v>
       </c>
-      <c r="E31" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>680</v>
+      <c r="E31" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1682</v>
       </c>
       <c r="F31" s="24">
         <v>0</v>
@@ -2231,22 +2228,22 @@
       <c r="H31" s="34"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="C32" s="22">
-        <v>44956</v>
+        <v>43886</v>
       </c>
       <c r="D32" s="4">
         <v>45546</v>
       </c>
-      <c r="E32" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>590</v>
+      <c r="E32" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1660</v>
       </c>
       <c r="F32" s="24">
         <v>0</v>
@@ -2255,22 +2252,22 @@
       <c r="H32" s="34"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C33" s="22">
-        <v>44874</v>
+        <v>43982</v>
       </c>
       <c r="D33" s="4">
         <v>45546</v>
       </c>
-      <c r="E33" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>672</v>
+      <c r="E33" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1564</v>
       </c>
       <c r="F33" s="24">
         <v>0</v>
@@ -2279,22 +2276,22 @@
       <c r="H33" s="34"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="C34" s="22">
-        <v>44918</v>
+        <v>43999</v>
       </c>
       <c r="D34" s="4">
         <v>45546</v>
       </c>
-      <c r="E34" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>628</v>
+      <c r="E34" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1547</v>
       </c>
       <c r="F34" s="24">
         <v>0</v>
@@ -2303,22 +2300,22 @@
       <c r="H34" s="34"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="C35" s="22">
-        <v>44060</v>
+        <v>44016</v>
       </c>
       <c r="D35" s="4">
         <v>45546</v>
       </c>
-      <c r="E35" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1486</v>
+      <c r="E35" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1530</v>
       </c>
       <c r="F35" s="24">
         <v>0</v>
@@ -2327,22 +2324,22 @@
       <c r="H35" s="34"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="22">
-        <v>44117</v>
+        <v>44018</v>
       </c>
       <c r="D36" s="4">
         <v>45546</v>
       </c>
-      <c r="E36" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1429</v>
+      <c r="E36" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1528</v>
       </c>
       <c r="F36" s="24">
         <v>0</v>
@@ -2351,22 +2348,22 @@
       <c r="H36" s="34"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C37" s="22">
-        <v>44128</v>
+        <v>44040</v>
       </c>
       <c r="D37" s="4">
         <v>45546</v>
       </c>
-      <c r="E37" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1418</v>
+      <c r="E37" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1506</v>
       </c>
       <c r="F37" s="24">
         <v>0</v>
@@ -2375,22 +2372,22 @@
       <c r="H37" s="34"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C38" s="22">
-        <v>44252</v>
+        <v>44051</v>
       </c>
       <c r="D38" s="4">
         <v>45546</v>
       </c>
-      <c r="E38" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1294</v>
+      <c r="E38" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1495</v>
       </c>
       <c r="F38" s="24">
         <v>0</v>
@@ -2399,22 +2396,22 @@
       <c r="H38" s="34"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C39" s="22">
-        <v>44254</v>
+        <v>44060</v>
       </c>
       <c r="D39" s="4">
         <v>45546</v>
       </c>
-      <c r="E39" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1292</v>
+      <c r="E39" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1486</v>
       </c>
       <c r="F39" s="24">
         <v>0</v>
@@ -2423,22 +2420,22 @@
       <c r="H39" s="34"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C40" s="22">
-        <v>44382</v>
+        <v>44082</v>
       </c>
       <c r="D40" s="4">
         <v>45546</v>
       </c>
-      <c r="E40" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1164</v>
+      <c r="E40" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1464</v>
       </c>
       <c r="F40" s="24">
         <v>0</v>
@@ -2447,22 +2444,22 @@
       <c r="H40" s="34"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C41" s="22">
-        <v>44406</v>
+        <v>44105</v>
       </c>
       <c r="D41" s="4">
         <v>45546</v>
       </c>
-      <c r="E41" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1140</v>
+      <c r="E41" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1441</v>
       </c>
       <c r="F41" s="24">
         <v>0</v>
@@ -2471,22 +2468,22 @@
       <c r="H41" s="34"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C42" s="22">
-        <v>44406</v>
+        <v>44106</v>
       </c>
       <c r="D42" s="4">
         <v>45546</v>
       </c>
-      <c r="E42" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1140</v>
+      <c r="E42" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1440</v>
       </c>
       <c r="F42" s="24">
         <v>0</v>
@@ -2495,22 +2492,22 @@
       <c r="H42" s="34"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C43" s="22">
-        <v>44525</v>
-      </c>
-      <c r="D43" s="32">
-        <v>45544.357870370368</v>
-      </c>
-      <c r="E43" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1019.3578703703679</v>
+        <v>44117</v>
+      </c>
+      <c r="D43" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E43" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1429</v>
       </c>
       <c r="F43" s="24">
         <v>0</v>
@@ -2519,22 +2516,22 @@
       <c r="H43" s="34"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C44" s="22">
-        <v>44602</v>
+        <v>44126</v>
       </c>
       <c r="D44" s="4">
         <v>45546</v>
       </c>
-      <c r="E44" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>944</v>
+      <c r="E44" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1420</v>
       </c>
       <c r="F44" s="24">
         <v>0</v>
@@ -2543,22 +2540,22 @@
       <c r="H44" s="34"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C45" s="22">
-        <v>44719</v>
+        <v>44128</v>
       </c>
       <c r="D45" s="4">
         <v>45546</v>
       </c>
-      <c r="E45" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>827</v>
+      <c r="E45" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1418</v>
       </c>
       <c r="F45" s="25">
         <v>0</v>
@@ -2567,22 +2564,22 @@
       <c r="H45" s="34"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C46" s="22">
-        <v>44752</v>
+        <v>44129</v>
       </c>
       <c r="D46" s="4">
         <v>45546</v>
       </c>
-      <c r="E46" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>794</v>
+      <c r="E46" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1417</v>
       </c>
       <c r="F46" s="25">
         <v>0</v>
@@ -2591,22 +2588,22 @@
       <c r="H46" s="34"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="C47" s="22">
-        <v>44778</v>
-      </c>
-      <c r="D47" s="32">
-        <v>45400.999976851854</v>
-      </c>
-      <c r="E47" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>622.99997685185372</v>
+        <v>44156</v>
+      </c>
+      <c r="D47" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E47" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1390</v>
       </c>
       <c r="F47" s="25">
         <v>0</v>
@@ -2615,22 +2612,22 @@
       <c r="H47" s="34"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
-        <v>46</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>49</v>
+        <v>5</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="C48" s="22">
-        <v>45100</v>
-      </c>
-      <c r="D48" s="32">
-        <v>45545.595462962963</v>
-      </c>
-      <c r="E48" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>445.59546296296321</v>
+        <v>44172</v>
+      </c>
+      <c r="D48" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E48" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1374</v>
       </c>
       <c r="F48" s="25">
         <v>0</v>
@@ -2639,22 +2636,22 @@
       <c r="H48" s="34"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C49" s="22">
-        <v>45200</v>
+        <v>44184</v>
       </c>
       <c r="D49" s="4">
         <v>45546</v>
       </c>
-      <c r="E49" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>346</v>
+      <c r="E49" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1362</v>
       </c>
       <c r="F49" s="25">
         <v>0</v>
@@ -2663,22 +2660,22 @@
       <c r="H49" s="34"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C50" s="22">
-        <v>44018</v>
+        <v>44194</v>
       </c>
       <c r="D50" s="4">
         <v>45546</v>
       </c>
-      <c r="E50" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1528</v>
+      <c r="E50" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1352</v>
       </c>
       <c r="F50" s="25">
         <v>0</v>
@@ -2687,22 +2684,22 @@
       <c r="H50" s="34"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C51" s="22">
-        <v>45118</v>
+        <v>44210</v>
       </c>
       <c r="D51" s="4">
         <v>45546</v>
       </c>
-      <c r="E51" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>428</v>
+      <c r="E51" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1336</v>
       </c>
       <c r="F51" s="25">
         <v>0</v>
@@ -2711,22 +2708,22 @@
       <c r="H51" s="34"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C52" s="22">
-        <v>43982</v>
+        <v>44250</v>
       </c>
       <c r="D52" s="4">
         <v>45546</v>
       </c>
-      <c r="E52" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1564</v>
+      <c r="E52" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1296</v>
       </c>
       <c r="F52" s="25">
         <v>0</v>
@@ -2735,7 +2732,7 @@
       <c r="H52" s="34"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <v>50</v>
       </c>
@@ -2748,7 +2745,7 @@
       <c r="D53" s="32">
         <v>45518.999826388892</v>
       </c>
-      <c r="E53" s="41">
+      <c r="E53" s="35">
         <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
         <v>1267.999826388892</v>
       </c>
@@ -2759,22 +2756,22 @@
       <c r="H53" s="34"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C54" s="22">
-        <v>42736</v>
+        <v>44252</v>
       </c>
       <c r="D54" s="4">
         <v>45546</v>
       </c>
-      <c r="E54" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2810</v>
+      <c r="E54" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1294</v>
       </c>
       <c r="F54" s="25">
         <v>0</v>
@@ -2783,22 +2780,22 @@
       <c r="H54" s="34"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C55" s="22">
-        <v>44910</v>
+        <v>44254</v>
       </c>
       <c r="D55" s="4">
         <v>45546</v>
       </c>
-      <c r="E55" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>636</v>
+      <c r="E55" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1292</v>
       </c>
       <c r="F55" s="25">
         <v>0</v>
@@ -2806,22 +2803,22 @@
       <c r="G55" s="2"/>
       <c r="H55" s="34"/>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="C56" s="22">
-        <v>44920</v>
+        <v>44275</v>
       </c>
       <c r="D56" s="32">
-        <v>45324.995092592595</v>
-      </c>
-      <c r="E56" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>404.99509259259503</v>
+        <v>45463.999884259261</v>
+      </c>
+      <c r="E56" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1188.9998842592613</v>
       </c>
       <c r="F56" s="25">
         <v>0</v>
@@ -2830,20 +2827,23 @@
       <c r="H56" s="34"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="D57" t="s">
-        <v>264</v>
-      </c>
-      <c r="E57" s="42"/>
+        <v>29</v>
+      </c>
+      <c r="C57" s="22">
+        <v>44282</v>
+      </c>
+      <c r="D57" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E57" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1264</v>
+      </c>
       <c r="F57" s="25">
         <v>0</v>
       </c>
@@ -2851,22 +2851,22 @@
       <c r="H57" s="34"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="14">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="C58" s="22">
-        <v>44105</v>
+        <v>44285</v>
       </c>
       <c r="D58" s="4">
         <v>45546</v>
       </c>
-      <c r="E58" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1441</v>
+      <c r="E58" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1261</v>
       </c>
       <c r="F58" s="25">
         <v>0</v>
@@ -2875,22 +2875,22 @@
       <c r="H58" s="34"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="14">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C59" s="22">
-        <v>44629</v>
+        <v>44313</v>
       </c>
       <c r="D59" s="4">
         <v>45546</v>
       </c>
-      <c r="E59" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>917</v>
+      <c r="E59" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1233</v>
       </c>
       <c r="F59" s="25">
         <v>0</v>
@@ -2899,22 +2899,22 @@
       <c r="H59" s="34"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="C60" s="22">
-        <v>43799</v>
-      </c>
-      <c r="D60" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E60" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1747</v>
+        <v>44336</v>
+      </c>
+      <c r="D60" s="32">
+        <v>45278.999942129631</v>
+      </c>
+      <c r="E60" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>942.99994212963065</v>
       </c>
       <c r="F60" s="25">
         <v>0</v>
@@ -2923,22 +2923,22 @@
       <c r="H60" s="34"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="14">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="C61" s="22">
-        <v>44126</v>
+        <v>44341</v>
       </c>
       <c r="D61" s="4">
         <v>45546</v>
       </c>
-      <c r="E61" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1420</v>
+      <c r="E61" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1205</v>
       </c>
       <c r="F61" s="25">
         <v>0</v>
@@ -2947,22 +2947,22 @@
       <c r="H61" s="34"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="14">
-        <v>59</v>
+        <v>143</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="C62" s="22">
-        <v>44184</v>
+        <v>44358</v>
       </c>
       <c r="D62" s="4">
         <v>45546</v>
       </c>
-      <c r="E62" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1362</v>
+      <c r="E62" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1188</v>
       </c>
       <c r="F62" s="25">
         <v>0</v>
@@ -2971,22 +2971,22 @@
       <c r="H62" s="34"/>
       <c r="J62" s="4"/>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="14">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C63" s="22">
-        <v>44210</v>
-      </c>
-      <c r="D63" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E63" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1336</v>
+        <v>44369</v>
+      </c>
+      <c r="D63" s="32">
+        <v>45476.941145833334</v>
+      </c>
+      <c r="E63" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1107.9411458333343</v>
       </c>
       <c r="F63" s="25">
         <v>0</v>
@@ -2995,22 +2995,22 @@
       <c r="H63" s="34"/>
       <c r="J63" s="4"/>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="14">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C64" s="22">
-        <v>44915</v>
+        <v>44375</v>
       </c>
       <c r="D64" s="4">
         <v>45546</v>
       </c>
-      <c r="E64" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>631</v>
+      <c r="E64" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1171</v>
       </c>
       <c r="F64" s="25">
         <v>0</v>
@@ -3019,22 +3019,22 @@
       <c r="H64" s="34"/>
       <c r="J64" s="4"/>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C65" s="22">
-        <v>44970</v>
+        <v>44382</v>
       </c>
       <c r="D65" s="4">
         <v>45546</v>
       </c>
-      <c r="E65" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>576</v>
+      <c r="E65" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1164</v>
       </c>
       <c r="F65" s="25">
         <v>0</v>
@@ -3043,22 +3043,22 @@
       <c r="H65" s="34"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C66" s="22">
-        <v>45209</v>
+        <v>44406</v>
       </c>
       <c r="D66" s="4">
         <v>45546</v>
       </c>
-      <c r="E66" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>337</v>
+      <c r="E66" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1140</v>
       </c>
       <c r="F66" s="25">
         <v>0</v>
@@ -3067,22 +3067,22 @@
       <c r="H66" s="34"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C67" s="22">
-        <v>44457</v>
+        <v>44406</v>
       </c>
       <c r="D67" s="4">
         <v>45546</v>
       </c>
-      <c r="E67" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1089</v>
+      <c r="E67" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1140</v>
       </c>
       <c r="F67" s="25">
         <v>0</v>
@@ -3091,22 +3091,22 @@
       <c r="H67" s="34"/>
       <c r="J67" s="4"/>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C68" s="22">
-        <v>44916</v>
+        <v>44406</v>
       </c>
       <c r="D68" s="4">
         <v>45546</v>
       </c>
-      <c r="E68" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>630</v>
+      <c r="E68" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1140</v>
       </c>
       <c r="F68" s="25">
         <v>0</v>
@@ -3115,22 +3115,22 @@
       <c r="H68" s="34"/>
       <c r="J68" s="4"/>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C69" s="22">
-        <v>44250</v>
-      </c>
-      <c r="D69" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E69" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1296</v>
+        <v>44414</v>
+      </c>
+      <c r="D69" s="32">
+        <v>45400.874641203707</v>
+      </c>
+      <c r="E69" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>986.87464120370714</v>
       </c>
       <c r="F69" s="25">
         <v>0</v>
@@ -3139,22 +3139,22 @@
       <c r="H69" s="34"/>
       <c r="J69" s="4"/>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C70" s="22">
-        <v>45106</v>
+        <v>44418</v>
       </c>
       <c r="D70" s="32">
-        <v>45539.996655092589</v>
-      </c>
-      <c r="E70" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>433.99665509258921</v>
+        <v>45468.999965277777</v>
+      </c>
+      <c r="E70" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1050.9999652777769</v>
       </c>
       <c r="F70" s="25">
         <v>0</v>
@@ -3163,22 +3163,22 @@
       <c r="H70" s="34"/>
       <c r="J70" s="4"/>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="C71" s="22">
-        <v>44758</v>
-      </c>
-      <c r="D71" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E71" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>788</v>
+        <v>44428</v>
+      </c>
+      <c r="D71" s="32">
+        <v>45396.999988425923</v>
+      </c>
+      <c r="E71" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>968.99998842592322</v>
       </c>
       <c r="F71" s="25">
         <v>0</v>
@@ -3187,22 +3187,22 @@
       <c r="H71" s="34"/>
       <c r="J71" s="4"/>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C72" s="22">
-        <v>44816</v>
-      </c>
-      <c r="D72" s="32">
-        <v>45499.857685185183</v>
-      </c>
-      <c r="E72" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>683.85768518518307</v>
+        <v>44432</v>
+      </c>
+      <c r="D72" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E72" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1114</v>
       </c>
       <c r="F72" s="25">
         <v>0</v>
@@ -3211,22 +3211,22 @@
       <c r="H72" s="34"/>
       <c r="J72" s="4"/>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C73" s="22">
-        <v>44846</v>
-      </c>
-      <c r="D73" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E73" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>700</v>
+        <v>44450</v>
+      </c>
+      <c r="D73" s="32">
+        <v>45325.999918981484</v>
+      </c>
+      <c r="E73" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>875.99991898148437</v>
       </c>
       <c r="F73" s="25">
         <v>0</v>
@@ -3235,22 +3235,22 @@
       <c r="H73" s="34"/>
       <c r="J73" s="4"/>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C74" s="22">
-        <v>43535</v>
+        <v>44457</v>
       </c>
       <c r="D74" s="4">
         <v>45546</v>
       </c>
-      <c r="E74" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2011</v>
+      <c r="E74" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1089</v>
       </c>
       <c r="F74" s="25">
         <v>0</v>
@@ -3259,22 +3259,22 @@
       <c r="H74" s="34"/>
       <c r="J74" s="4"/>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C75" s="22">
-        <v>45104</v>
+        <v>44460</v>
       </c>
       <c r="D75" s="32">
-        <v>45386.999872685185</v>
-      </c>
-      <c r="E75" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>282.99987268518453</v>
+        <v>45278.999930555554</v>
+      </c>
+      <c r="E75" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>818.99993055555387</v>
       </c>
       <c r="F75" s="25">
         <v>0</v>
@@ -3283,22 +3283,22 @@
       <c r="H75" s="34"/>
       <c r="J75" s="4"/>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="C76" s="22">
-        <v>45016</v>
+        <v>44461</v>
       </c>
       <c r="D76" s="4">
         <v>45546</v>
       </c>
-      <c r="E76" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>530</v>
+      <c r="E76" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1085</v>
       </c>
       <c r="F76" s="26">
         <v>0</v>
@@ -3307,22 +3307,22 @@
       <c r="H76" s="34"/>
       <c r="J76" s="4"/>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="14">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="C77" s="22">
-        <v>44734</v>
+        <v>44493</v>
       </c>
       <c r="D77" s="4">
         <v>45546</v>
       </c>
-      <c r="E77" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>812</v>
+      <c r="E77" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1053</v>
       </c>
       <c r="F77" s="26">
         <v>0</v>
@@ -3331,22 +3331,22 @@
       <c r="H77" s="34"/>
       <c r="J77" s="4"/>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="14">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="C78" s="22">
-        <v>45007</v>
-      </c>
-      <c r="D78" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E78" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>539</v>
+        <v>44525</v>
+      </c>
+      <c r="D78" s="32">
+        <v>45544.357870370368</v>
+      </c>
+      <c r="E78" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1019.3578703703679</v>
       </c>
       <c r="F78" s="26">
         <v>0</v>
@@ -3355,22 +3355,22 @@
       <c r="H78" s="34"/>
       <c r="J78" s="4"/>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="14">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="C79" s="22">
-        <v>45046</v>
+        <v>44534</v>
       </c>
       <c r="D79" s="4">
         <v>45546</v>
       </c>
-      <c r="E79" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>500</v>
+      <c r="E79" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>1012</v>
       </c>
       <c r="F79" s="26">
         <v>0</v>
@@ -3379,22 +3379,22 @@
       <c r="H79" s="34"/>
       <c r="J79" s="4"/>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="14">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C80" s="22">
-        <v>45060</v>
+        <v>44598</v>
       </c>
       <c r="D80" s="4">
         <v>45546</v>
       </c>
-      <c r="E80" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>486</v>
+      <c r="E80" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>948</v>
       </c>
       <c r="F80" s="26">
         <v>0</v>
@@ -3403,22 +3403,22 @@
       <c r="H80" s="34"/>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="14">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C81" s="22">
-        <v>43736</v>
+        <v>44602</v>
       </c>
       <c r="D81" s="4">
         <v>45546</v>
       </c>
-      <c r="E81" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1810</v>
+      <c r="E81" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>944</v>
       </c>
       <c r="F81" s="26">
         <v>0</v>
@@ -3427,22 +3427,22 @@
       <c r="H81" s="34"/>
       <c r="J81" s="4"/>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C82" s="22">
-        <v>43349</v>
-      </c>
-      <c r="D82" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E82" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2197</v>
+        <v>44620</v>
+      </c>
+      <c r="D82" s="32">
+        <v>45283.999884259261</v>
+      </c>
+      <c r="E82" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>663.99988425926131</v>
       </c>
       <c r="F82" s="26">
         <v>0</v>
@@ -3451,22 +3451,22 @@
       <c r="H82" s="34"/>
       <c r="J82" s="4"/>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="14">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C83" s="22">
-        <v>44375</v>
+        <v>44629</v>
       </c>
       <c r="D83" s="4">
         <v>45546</v>
       </c>
-      <c r="E83" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1171</v>
+      <c r="E83" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>917</v>
       </c>
       <c r="F83" s="26">
         <v>0</v>
@@ -3475,46 +3475,46 @@
       <c r="H83" s="34"/>
       <c r="J83" s="4"/>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="C84" s="22">
-        <v>45306</v>
-      </c>
-      <c r="D84" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E84" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>240</v>
+        <v>44680</v>
+      </c>
+      <c r="D84" s="32">
+        <v>45525.999895833331</v>
+      </c>
+      <c r="E84" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>845.99989583333081</v>
       </c>
       <c r="F84" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="34"/>
       <c r="J84" s="4"/>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="14">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C85" s="22">
-        <v>44369</v>
-      </c>
-      <c r="D85" s="32">
-        <v>45476.941145833334</v>
-      </c>
-      <c r="E85" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1107.9411458333343</v>
+        <v>44680</v>
+      </c>
+      <c r="D85" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E85" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>866</v>
       </c>
       <c r="F85" s="26">
         <v>0</v>
@@ -3523,22 +3523,22 @@
       <c r="H85" s="34"/>
       <c r="J85" s="4"/>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="C86" s="22">
-        <v>44406</v>
+        <v>44719</v>
       </c>
       <c r="D86" s="4">
         <v>45546</v>
       </c>
-      <c r="E86" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1140</v>
+      <c r="E86" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>827</v>
       </c>
       <c r="F86" s="26">
         <v>0</v>
@@ -3547,22 +3547,22 @@
       <c r="H86" s="34"/>
       <c r="J86" s="4"/>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="14">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C87" s="22">
-        <v>44432</v>
+        <v>44734</v>
       </c>
       <c r="D87" s="4">
         <v>45546</v>
       </c>
-      <c r="E87" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1114</v>
+      <c r="E87" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>812</v>
       </c>
       <c r="F87" s="26">
         <v>0</v>
@@ -3571,22 +3571,22 @@
       <c r="H87" s="34"/>
       <c r="J87" s="4"/>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C88" s="22">
-        <v>44460</v>
-      </c>
-      <c r="D88" s="32">
-        <v>45278.999930555554</v>
-      </c>
-      <c r="E88" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>818.99993055555387</v>
+        <v>44735</v>
+      </c>
+      <c r="D88" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E88" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>811</v>
       </c>
       <c r="F88" s="26">
         <v>0</v>
@@ -3595,22 +3595,22 @@
       <c r="H88" s="34"/>
       <c r="J88" s="4"/>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="C89" s="22">
-        <v>43357</v>
+        <v>44738</v>
       </c>
       <c r="D89" s="4">
         <v>45546</v>
       </c>
-      <c r="E89" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2189</v>
+      <c r="E89" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>808</v>
       </c>
       <c r="F89" s="26">
         <v>0</v>
@@ -3619,22 +3619,22 @@
       <c r="H89" s="34"/>
       <c r="J89" s="4"/>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="C90" s="22">
-        <v>45092</v>
-      </c>
-      <c r="D90" s="32">
-        <v>45531.999537037038</v>
-      </c>
-      <c r="E90" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>439.99953703703795</v>
+        <v>44752</v>
+      </c>
+      <c r="D90" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E90" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>794</v>
       </c>
       <c r="F90" s="26">
         <v>0</v>
@@ -3643,22 +3643,22 @@
       <c r="H90" s="34"/>
       <c r="J90" s="4"/>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="14">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C91" s="22">
-        <v>44828</v>
+        <v>44758</v>
       </c>
       <c r="D91" s="4">
         <v>45546</v>
       </c>
-      <c r="E91" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>718</v>
+      <c r="E91" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>788</v>
       </c>
       <c r="F91" s="26">
         <v>0</v>
@@ -3667,22 +3667,22 @@
       <c r="H91" s="34"/>
       <c r="J91" s="4"/>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="14">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C92" s="22">
-        <v>44844</v>
-      </c>
-      <c r="D92" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E92" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>702</v>
+        <v>44778</v>
+      </c>
+      <c r="D92" s="32">
+        <v>45400.999976851854</v>
+      </c>
+      <c r="E92" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>622.99997685185372</v>
       </c>
       <c r="F92" s="26">
         <v>0</v>
@@ -3691,22 +3691,22 @@
       <c r="H92" s="34"/>
       <c r="J92" s="4"/>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="14">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>92</v>
+        <v>3</v>
       </c>
       <c r="C93" s="22">
-        <v>44916</v>
-      </c>
-      <c r="D93" s="32">
-        <v>45510.999884259261</v>
-      </c>
-      <c r="E93" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>594.99988425926131</v>
+        <v>44783</v>
+      </c>
+      <c r="D93" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E93" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>763</v>
       </c>
       <c r="F93" s="26">
         <v>0</v>
@@ -3714,22 +3714,22 @@
       <c r="G93" s="2"/>
       <c r="H93" s="34"/>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="14">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C94" s="22">
-        <v>45004</v>
+        <v>44798</v>
       </c>
       <c r="D94" s="4">
         <v>45546</v>
       </c>
-      <c r="E94" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>542</v>
+      <c r="E94" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>748</v>
       </c>
       <c r="F94" s="26">
         <v>0</v>
@@ -3738,22 +3738,22 @@
       <c r="H94" s="34"/>
       <c r="J94" s="4"/>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="14">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="C95" s="22">
-        <v>45007</v>
-      </c>
-      <c r="D95" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E95" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>539</v>
+        <v>44816</v>
+      </c>
+      <c r="D95" s="32">
+        <v>45499.857685185183</v>
+      </c>
+      <c r="E95" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>683.85768518518307</v>
       </c>
       <c r="F95" s="26">
         <v>0</v>
@@ -3762,20 +3762,23 @@
       <c r="H95" s="34"/>
       <c r="J95" s="4"/>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="14">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="D96" t="s">
-        <v>264</v>
-      </c>
-      <c r="E96" s="42"/>
+        <v>140</v>
+      </c>
+      <c r="C96" s="22">
+        <v>44819</v>
+      </c>
+      <c r="D96" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E96" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>727</v>
+      </c>
       <c r="F96" s="26">
         <v>0</v>
       </c>
@@ -3783,22 +3786,22 @@
       <c r="H96" s="34"/>
       <c r="J96" s="4"/>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="14">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C97" s="22">
-        <v>43650</v>
-      </c>
-      <c r="D97" s="32">
-        <v>45542.998993055553</v>
-      </c>
-      <c r="E97" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1892.998993055553</v>
+        <v>44828</v>
+      </c>
+      <c r="D97" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E97" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>718</v>
       </c>
       <c r="F97" s="27">
         <v>0</v>
@@ -3807,22 +3810,22 @@
       <c r="H97" s="34"/>
       <c r="J97" s="4"/>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="14">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C98" s="22">
-        <v>43729</v>
+        <v>44844</v>
       </c>
       <c r="D98" s="4">
         <v>45546</v>
       </c>
-      <c r="E98" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1817</v>
+      <c r="E98" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>702</v>
       </c>
       <c r="F98" s="27">
         <v>0</v>
@@ -3831,22 +3834,22 @@
       <c r="H98" s="34"/>
       <c r="J98" s="4"/>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="14">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C99" s="22">
-        <v>43886</v>
+        <v>44846</v>
       </c>
       <c r="D99" s="4">
         <v>45546</v>
       </c>
-      <c r="E99" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1660</v>
+      <c r="E99" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>700</v>
       </c>
       <c r="F99" s="27">
         <v>0</v>
@@ -3855,22 +3858,22 @@
       <c r="H99" s="34"/>
       <c r="J99" s="4"/>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="14">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C100" s="22">
-        <v>43999</v>
+        <v>44855</v>
       </c>
       <c r="D100" s="4">
         <v>45546</v>
       </c>
-      <c r="E100" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1547</v>
+      <c r="E100" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>691</v>
       </c>
       <c r="F100" s="27">
         <v>0</v>
@@ -3881,20 +3884,20 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="14">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="C101" s="22">
-        <v>43568</v>
+        <v>44859</v>
       </c>
       <c r="D101" s="4">
         <v>45546</v>
       </c>
-      <c r="E101" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1978</v>
+      <c r="E101" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>687</v>
       </c>
       <c r="F101" s="27">
         <v>0</v>
@@ -3903,22 +3906,22 @@
       <c r="H101" s="34"/>
       <c r="J101" s="4"/>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="14">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="C102" s="22">
-        <v>44082</v>
+        <v>44866</v>
       </c>
       <c r="D102" s="4">
         <v>45546</v>
       </c>
-      <c r="E102" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1464</v>
+      <c r="E102" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>680</v>
       </c>
       <c r="F102" s="27">
         <v>0</v>
@@ -3927,22 +3930,22 @@
       <c r="H102" s="34"/>
       <c r="J102" s="4"/>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="14">
-        <v>99</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>102</v>
+        <v>1</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="C103" s="22">
-        <v>44129</v>
+        <v>44874</v>
       </c>
       <c r="D103" s="4">
         <v>45546</v>
       </c>
-      <c r="E103" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1417</v>
+      <c r="E103" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>672</v>
       </c>
       <c r="F103" s="27">
         <v>0</v>
@@ -3951,22 +3954,22 @@
       <c r="H103" s="34"/>
       <c r="J103" s="4"/>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="14">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="C104" s="22">
-        <v>44156</v>
+        <v>44874</v>
       </c>
       <c r="D104" s="4">
         <v>45546</v>
       </c>
-      <c r="E104" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1390</v>
+      <c r="E104" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>672</v>
       </c>
       <c r="F104" s="27">
         <v>0</v>
@@ -3975,22 +3978,22 @@
       <c r="H104" s="34"/>
       <c r="J104" s="4"/>
     </row>
-    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="14">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="C105" s="22">
-        <v>44275</v>
-      </c>
-      <c r="D105" s="32">
-        <v>45463.999884259261</v>
-      </c>
-      <c r="E105" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1188.9998842592613</v>
+        <v>44910</v>
+      </c>
+      <c r="D105" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E105" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>636</v>
       </c>
       <c r="F105" s="27">
         <v>0</v>
@@ -3999,22 +4002,22 @@
       <c r="H105" s="34"/>
       <c r="J105" s="4"/>
     </row>
-    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="14">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C106" s="22">
-        <v>44341</v>
+        <v>44915</v>
       </c>
       <c r="D106" s="4">
         <v>45546</v>
       </c>
-      <c r="E106" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1205</v>
+      <c r="E106" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>631</v>
       </c>
       <c r="F106" s="27">
         <v>0</v>
@@ -4023,22 +4026,22 @@
       <c r="H106" s="34"/>
       <c r="J106" s="4"/>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="14">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="C107" s="22">
-        <v>44598</v>
+        <v>44916</v>
       </c>
       <c r="D107" s="4">
         <v>45546</v>
       </c>
-      <c r="E107" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>948</v>
+      <c r="E107" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>630</v>
       </c>
       <c r="F107" s="27">
         <v>0</v>
@@ -4047,22 +4050,22 @@
       <c r="H107" s="34"/>
       <c r="J107" s="4"/>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="14">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C108" s="22">
-        <v>44620</v>
+        <v>44916</v>
       </c>
       <c r="D108" s="32">
-        <v>45283.999884259261</v>
-      </c>
-      <c r="E108" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>663.99988425926131</v>
+        <v>45510.999884259261</v>
+      </c>
+      <c r="E108" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>594.99988425926131</v>
       </c>
       <c r="F108" s="27">
         <v>0</v>
@@ -4070,22 +4073,22 @@
       <c r="G108" s="2"/>
       <c r="H108" s="34"/>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="14">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="C109" s="22">
-        <v>44680</v>
+        <v>44918</v>
       </c>
       <c r="D109" s="4">
         <v>45546</v>
       </c>
-      <c r="E109" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>866</v>
+      <c r="E109" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>628</v>
       </c>
       <c r="F109" s="27">
         <v>0</v>
@@ -4094,22 +4097,22 @@
       <c r="H109" s="34"/>
       <c r="J109" s="4"/>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="14">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="C110" s="22">
-        <v>44798</v>
-      </c>
-      <c r="D110" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E110" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>748</v>
+        <v>44920</v>
+      </c>
+      <c r="D110" s="32">
+        <v>45324.995092592595</v>
+      </c>
+      <c r="E110" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>404.99509259259503</v>
       </c>
       <c r="F110" s="27">
         <v>0</v>
@@ -4118,20 +4121,23 @@
       <c r="H110" s="34"/>
       <c r="J110" s="4"/>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="14">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="D111" t="s">
-        <v>264</v>
-      </c>
-      <c r="E111" s="42"/>
+        <v>21</v>
+      </c>
+      <c r="C111" s="22">
+        <v>44923</v>
+      </c>
+      <c r="D111" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E111" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>623</v>
+      </c>
       <c r="F111" s="27">
         <v>0</v>
       </c>
@@ -4139,22 +4145,22 @@
       <c r="H111" s="34"/>
       <c r="J111" s="4"/>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="14">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C112" s="22">
-        <v>42940</v>
+        <v>44932</v>
       </c>
       <c r="D112" s="4">
         <v>45546</v>
       </c>
-      <c r="E112" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2606</v>
+      <c r="E112" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>614</v>
       </c>
       <c r="F112" s="27">
         <v>0</v>
@@ -4163,22 +4169,22 @@
       <c r="H112" s="34"/>
       <c r="J112" s="4"/>
     </row>
-    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="14">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="C113" s="22">
-        <v>43419</v>
+        <v>44943</v>
       </c>
       <c r="D113" s="4">
         <v>45546</v>
       </c>
-      <c r="E113" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2127</v>
+      <c r="E113" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>603</v>
       </c>
       <c r="F113" s="27">
         <v>0</v>
@@ -4187,22 +4193,22 @@
       <c r="H113" s="34"/>
       <c r="J113" s="4"/>
     </row>
-    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="14">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="C114" s="22">
-        <v>44428</v>
-      </c>
-      <c r="D114" s="32">
-        <v>45396.999988425923</v>
-      </c>
-      <c r="E114" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>968.99998842592322</v>
+        <v>44956</v>
+      </c>
+      <c r="D114" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E114" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>590</v>
       </c>
       <c r="F114" s="27">
         <v>0</v>
@@ -4211,22 +4217,22 @@
       <c r="H114" s="34"/>
       <c r="J114" s="4"/>
     </row>
-    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="14">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="C115" s="22">
-        <v>44855</v>
+        <v>44970</v>
       </c>
       <c r="D115" s="4">
         <v>45546</v>
       </c>
-      <c r="E115" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>691</v>
+      <c r="E115" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>576</v>
       </c>
       <c r="F115" s="27">
         <v>0</v>
@@ -4235,22 +4241,22 @@
       <c r="H115" s="34"/>
       <c r="J115" s="4"/>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="14">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="C116" s="22">
-        <v>44932</v>
+        <v>44981</v>
       </c>
       <c r="D116" s="4">
         <v>45546</v>
       </c>
-      <c r="E116" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>614</v>
+      <c r="E116" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>565</v>
       </c>
       <c r="F116" s="27">
         <v>0</v>
@@ -4259,22 +4265,22 @@
       <c r="H116" s="34"/>
       <c r="J116" s="4"/>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="14">
-        <v>110</v>
-      </c>
-      <c r="B117" s="10" t="s">
-        <v>113</v>
+        <v>2</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="C117" s="22">
-        <v>44051</v>
+        <v>44986</v>
       </c>
       <c r="D117" s="4">
         <v>45546</v>
       </c>
-      <c r="E117" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1495</v>
+      <c r="E117" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>560</v>
       </c>
       <c r="F117" s="27">
         <v>0</v>
@@ -4283,22 +4289,22 @@
       <c r="H117" s="34"/>
       <c r="J117" s="4"/>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="14">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="C118" s="22">
-        <v>45153</v>
+        <v>45004</v>
       </c>
       <c r="D118" s="4">
         <v>45546</v>
       </c>
-      <c r="E118" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>393</v>
+      <c r="E118" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>542</v>
       </c>
       <c r="F118" s="29">
         <v>0</v>
@@ -4307,22 +4313,22 @@
       <c r="H118" s="34"/>
       <c r="J118" s="4"/>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="C119" s="22">
-        <v>44450</v>
-      </c>
-      <c r="D119" s="32">
-        <v>45325.999918981484</v>
-      </c>
-      <c r="E119" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>875.99991898148437</v>
+        <v>45007</v>
+      </c>
+      <c r="D119" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E119" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>539</v>
       </c>
       <c r="F119" s="29">
         <v>0</v>
@@ -4331,22 +4337,22 @@
       <c r="H119" s="34"/>
       <c r="J119" s="4"/>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C120" s="22">
-        <v>43487</v>
+        <v>45007</v>
       </c>
       <c r="D120" s="4">
         <v>45546</v>
       </c>
-      <c r="E120" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2059</v>
+      <c r="E120" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>539</v>
       </c>
       <c r="F120" s="29">
         <v>0</v>
@@ -4355,22 +4361,22 @@
       <c r="H120" s="34"/>
       <c r="J120" s="4"/>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="14">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="C121" s="22">
-        <v>45083</v>
+        <v>45016</v>
       </c>
       <c r="D121" s="4">
         <v>45546</v>
       </c>
-      <c r="E121" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>463</v>
+      <c r="E121" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>530</v>
       </c>
       <c r="F121" s="29">
         <v>0</v>
@@ -4379,22 +4385,22 @@
       <c r="H121" s="34"/>
       <c r="J121" s="4"/>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C122" s="22">
-        <v>44493</v>
+        <v>45033</v>
       </c>
       <c r="D122" s="4">
         <v>45546</v>
       </c>
-      <c r="E122" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1053</v>
+      <c r="E122" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>513</v>
       </c>
       <c r="F122" s="29">
         <v>0</v>
@@ -4403,22 +4409,22 @@
       <c r="H122" s="34"/>
       <c r="J122" s="4"/>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="14">
-        <v>119</v>
-      </c>
-      <c r="B123" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C123" s="22">
-        <v>44414</v>
+        <v>45040</v>
       </c>
       <c r="D123" s="32">
-        <v>45400.874641203707</v>
-      </c>
-      <c r="E123" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>986.87464120370714</v>
+        <v>45407.999849537038</v>
+      </c>
+      <c r="E123" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>367.99984953703824</v>
       </c>
       <c r="F123" s="29">
         <v>0</v>
@@ -4427,22 +4433,22 @@
       <c r="H123" s="34"/>
       <c r="J123" s="4"/>
     </row>
-    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="14">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="C124" s="22">
-        <v>44783</v>
+        <v>45046</v>
       </c>
       <c r="D124" s="4">
         <v>45546</v>
       </c>
-      <c r="E124" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>763</v>
+      <c r="E124" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>500</v>
       </c>
       <c r="F124" s="29">
         <v>0</v>
@@ -4451,22 +4457,22 @@
       <c r="H124" s="34"/>
       <c r="J124" s="4"/>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="14">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="C125" s="22">
-        <v>43245</v>
+        <v>45060</v>
       </c>
       <c r="D125" s="4">
         <v>45546</v>
       </c>
-      <c r="E125" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2301</v>
+      <c r="E125" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>486</v>
       </c>
       <c r="F125" s="29">
         <v>0</v>
@@ -4475,22 +4481,22 @@
       <c r="H125" s="34"/>
       <c r="J125" s="4"/>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="14">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="C126" s="22">
-        <v>43329</v>
+        <v>45063</v>
       </c>
       <c r="D126" s="4">
         <v>45546</v>
       </c>
-      <c r="E126" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2217</v>
+      <c r="E126" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>483</v>
       </c>
       <c r="F126" s="29">
         <v>0</v>
@@ -4499,22 +4505,22 @@
       <c r="H126" s="34"/>
       <c r="J126" s="4"/>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="14">
-        <v>124</v>
-      </c>
-      <c r="B127" s="10" t="s">
-        <v>123</v>
+        <v>3</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C127" s="22">
-        <v>44285</v>
-      </c>
-      <c r="D127" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E127" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1261</v>
+        <v>45067</v>
+      </c>
+      <c r="D127" s="32">
+        <v>45344.902569444443</v>
+      </c>
+      <c r="E127" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>277.90256944444263</v>
       </c>
       <c r="F127" s="30">
         <v>0</v>
@@ -4523,22 +4529,22 @@
       <c r="H127" s="34"/>
       <c r="J127" s="4"/>
     </row>
-    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="14">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C128" s="22">
-        <v>44735</v>
+        <v>45083</v>
       </c>
       <c r="D128" s="4">
         <v>45546</v>
       </c>
-      <c r="E128" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>811</v>
+      <c r="E128" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>463</v>
       </c>
       <c r="F128" s="30">
         <v>0</v>
@@ -4547,22 +4553,22 @@
       <c r="H128" s="34"/>
       <c r="J128" s="4"/>
     </row>
-    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="14">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="C129" s="22">
-        <v>44016</v>
-      </c>
-      <c r="D129" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E129" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1530</v>
+        <v>45092</v>
+      </c>
+      <c r="D129" s="32">
+        <v>45531.999537037038</v>
+      </c>
+      <c r="E129" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>439.99953703703795</v>
       </c>
       <c r="F129" s="30">
         <v>0</v>
@@ -4571,22 +4577,22 @@
       <c r="H129" s="34"/>
       <c r="J129" s="4"/>
     </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="14">
-        <v>126</v>
+        <v>46</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>125</v>
+        <v>49</v>
       </c>
       <c r="C130" s="22">
-        <v>42866</v>
-      </c>
-      <c r="D130" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E130" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2680</v>
+        <v>45100</v>
+      </c>
+      <c r="D130" s="32">
+        <v>45545.595462962963</v>
+      </c>
+      <c r="E130" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>445.59546296296321</v>
       </c>
       <c r="F130" s="30">
         <v>0</v>
@@ -4595,22 +4601,22 @@
       <c r="H130" s="34"/>
       <c r="J130" s="4"/>
     </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="14">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="C131" s="22">
-        <v>45033</v>
+        <v>45104</v>
       </c>
       <c r="D131" s="4">
         <v>45546</v>
       </c>
-      <c r="E131" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>513</v>
+      <c r="E131" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>442</v>
       </c>
       <c r="F131" s="30">
         <v>0</v>
@@ -4619,22 +4625,22 @@
       <c r="H131" s="34"/>
       <c r="J131" s="4"/>
     </row>
-    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="14">
-        <v>128</v>
+        <v>72</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="C132" s="22">
-        <v>43864</v>
-      </c>
-      <c r="D132" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E132" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1682</v>
+        <v>45104</v>
+      </c>
+      <c r="D132" s="32">
+        <v>45386.999872685185</v>
+      </c>
+      <c r="E132" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>282.99987268518453</v>
       </c>
       <c r="F132" s="14">
         <v>0</v>
@@ -4643,22 +4649,22 @@
       <c r="H132" s="34"/>
       <c r="J132" s="4"/>
     </row>
-    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="14">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="C133" s="22">
-        <v>43621</v>
-      </c>
-      <c r="D133" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E133" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1925</v>
+        <v>45106</v>
+      </c>
+      <c r="D133" s="32">
+        <v>45539.996655092589</v>
+      </c>
+      <c r="E133" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>433.99665509258921</v>
       </c>
       <c r="F133" s="30">
         <v>0</v>
@@ -4667,22 +4673,22 @@
       <c r="H133" s="34"/>
       <c r="J133" s="4"/>
     </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="14">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="C134" s="22">
-        <v>44336</v>
-      </c>
-      <c r="D134" s="32">
-        <v>45278.999942129631</v>
-      </c>
-      <c r="E134" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>942.99994212963065</v>
+        <v>45118</v>
+      </c>
+      <c r="D134" s="4">
+        <v>45546</v>
+      </c>
+      <c r="E134" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>428</v>
       </c>
       <c r="F134" s="30">
         <v>0</v>
@@ -4691,22 +4697,22 @@
       <c r="H134" s="34"/>
       <c r="J134" s="4"/>
     </row>
-    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="14">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
       <c r="C135" s="22">
-        <v>42403</v>
+        <v>45124</v>
       </c>
       <c r="D135" s="4">
         <v>45546</v>
       </c>
-      <c r="E135" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>3143</v>
+      <c r="E135" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>422</v>
       </c>
       <c r="F135" s="30">
         <v>0</v>
@@ -4715,22 +4721,22 @@
       <c r="H135" s="34"/>
       <c r="J135" s="4"/>
     </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="14">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="C136" s="22">
-        <v>41049</v>
+        <v>45136</v>
       </c>
       <c r="D136" s="4">
         <v>45546</v>
       </c>
-      <c r="E136" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>4497</v>
+      <c r="E136" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>410</v>
       </c>
       <c r="F136" s="30">
         <v>0</v>
@@ -4739,22 +4745,22 @@
       <c r="H136" s="34"/>
       <c r="J136" s="4"/>
     </row>
-    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="14">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C137" s="22">
-        <v>41674</v>
+        <v>45153</v>
       </c>
       <c r="D137" s="4">
         <v>45546</v>
       </c>
-      <c r="E137" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>3872</v>
+      <c r="E137" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>393</v>
       </c>
       <c r="F137" s="30">
         <v>0</v>
@@ -4763,22 +4769,22 @@
       <c r="H137" s="34"/>
       <c r="J137" s="4"/>
     </row>
-    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="14">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>133</v>
+        <v>50</v>
       </c>
       <c r="C138" s="22">
-        <v>44859</v>
+        <v>45200</v>
       </c>
       <c r="D138" s="4">
         <v>45546</v>
       </c>
-      <c r="E138" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>687</v>
+      <c r="E138" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>346</v>
       </c>
       <c r="F138" s="30">
         <v>0</v>
@@ -4787,22 +4793,22 @@
       <c r="H138" s="34"/>
       <c r="J138" s="4"/>
     </row>
-    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="14">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>134</v>
+        <v>66</v>
       </c>
       <c r="C139" s="22">
-        <v>44981</v>
+        <v>45209</v>
       </c>
       <c r="D139" s="4">
         <v>45546</v>
       </c>
-      <c r="E139" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>565</v>
+      <c r="E139" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>337</v>
       </c>
       <c r="F139" s="30">
         <v>0</v>
@@ -4811,47 +4817,44 @@
       <c r="H139" s="34"/>
       <c r="J139" s="4"/>
     </row>
-    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="14">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C140" s="22">
-        <v>44313</v>
+        <v>45306</v>
       </c>
       <c r="D140" s="4">
         <v>45546</v>
       </c>
-      <c r="E140" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1233</v>
+      <c r="E140" s="35">
+        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
+        <v>240</v>
       </c>
       <c r="F140" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140" s="2"/>
       <c r="H140" s="34"/>
       <c r="J140" s="4"/>
     </row>
-    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="14">
-        <v>137</v>
+        <v>17</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C141" s="22">
-        <v>43433</v>
-      </c>
-      <c r="D141" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E141" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>2113</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D141" t="s">
+        <v>264</v>
+      </c>
+      <c r="E141" s="36"/>
       <c r="F141" s="30">
         <v>0</v>
       </c>
@@ -4859,23 +4862,20 @@
       <c r="H141" s="34"/>
       <c r="J141" s="4"/>
     </row>
-    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="14">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C142" s="22">
-        <v>43572</v>
-      </c>
-      <c r="D142" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E142" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1974</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C142" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D142" t="s">
+        <v>264</v>
+      </c>
+      <c r="E142" s="36"/>
       <c r="F142" s="30">
         <v>0</v>
       </c>
@@ -4883,23 +4883,20 @@
       <c r="H142" s="34"/>
       <c r="J142" s="4"/>
     </row>
-    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="14">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C143" s="22">
-        <v>45063</v>
-      </c>
-      <c r="D143" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E143" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>483</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D143" t="s">
+        <v>264</v>
+      </c>
+      <c r="E143" s="36"/>
       <c r="F143" s="30">
         <v>0</v>
       </c>
@@ -4907,23 +4904,20 @@
       <c r="H143" s="34"/>
       <c r="J143" s="4"/>
     </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="14">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C144" s="22">
-        <v>43612</v>
-      </c>
-      <c r="D144" s="4">
-        <v>45546</v>
-      </c>
-      <c r="E144" s="41">
-        <f>Table3[[#This Row],[fecha_ultimo_reporte]]-Table3[[#This Row],[inicio]]</f>
-        <v>1934</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="D144" t="s">
+        <v>264</v>
+      </c>
+      <c r="E144" s="36"/>
       <c r="F144" s="30">
         <v>0</v>
       </c>
@@ -5350,11 +5344,11 @@
       <c r="H1" t="s">
         <v>233</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -5448,7 +5442,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="38">
         <v>2</v>
       </c>
       <c r="K4" t="s">
@@ -5483,7 +5477,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="J5" s="36"/>
+      <c r="J5" s="38"/>
       <c r="K5" t="s">
         <v>241</v>
       </c>
@@ -5516,7 +5510,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J6" s="36"/>
+      <c r="J6" s="38"/>
       <c r="K6" t="s">
         <v>234</v>
       </c>
@@ -5549,7 +5543,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J7" s="36"/>
+      <c r="J7" s="38"/>
       <c r="K7" t="s">
         <v>242</v>
       </c>
@@ -5681,10 +5675,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="41">
         <f>L14+L29</f>
         <v>4.2859356589977011</v>
       </c>
@@ -5714,8 +5708,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="42"/>
       <c r="E13" t="s">
         <v>190</v>
       </c>
@@ -5795,11 +5789,11 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
@@ -5839,7 +5833,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J18" s="36">
+      <c r="J18" s="38">
         <v>1</v>
       </c>
       <c r="K18" t="s">
@@ -5864,7 +5858,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J19" s="36"/>
+      <c r="J19" s="38"/>
       <c r="K19" t="s">
         <v>248</v>
       </c>
@@ -5888,7 +5882,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J20" s="36"/>
+      <c r="J20" s="38"/>
       <c r="K20" t="s">
         <v>250</v>
       </c>
@@ -5912,7 +5906,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J21" s="36"/>
+      <c r="J21" s="38"/>
       <c r="K21" t="s">
         <v>251</v>
       </c>
@@ -5936,7 +5930,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J22" s="36">
+      <c r="J22" s="38">
         <v>2</v>
       </c>
       <c r="K22" s="20" t="s">
@@ -5961,7 +5955,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J23" s="36"/>
+      <c r="J23" s="38"/>
       <c r="K23" t="s">
         <v>253</v>
       </c>
@@ -5985,7 +5979,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J24" s="36"/>
+      <c r="J24" s="38"/>
       <c r="K24" t="s">
         <v>254</v>
       </c>
@@ -6009,7 +6003,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J25" s="36"/>
+      <c r="J25" s="38"/>
       <c r="K25" t="s">
         <v>255</v>
       </c>
@@ -6033,7 +6027,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J26" s="36"/>
+      <c r="J26" s="38"/>
       <c r="K26" t="s">
         <v>256</v>
       </c>
@@ -6057,7 +6051,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J27" s="36"/>
+      <c r="J27" s="38"/>
       <c r="K27" t="s">
         <v>257</v>
       </c>
@@ -6081,7 +6075,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J28" s="36"/>
+      <c r="J28" s="38"/>
       <c r="K28" t="s">
         <v>260</v>
       </c>
@@ -6105,7 +6099,7 @@
         <f>VLOOKUP(campos[[#This Row],[tipo_dato]],datos[],3,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="J29" s="36"/>
+      <c r="J29" s="38"/>
       <c r="K29" t="s">
         <v>261</v>
       </c>

</xml_diff>

<commit_message>
sume todas las variables de Wunder
</commit_message>
<xml_diff>
--- a/info_wunder.xlsx
+++ b/info_wunder.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\tecnicatura_ia\adscripcion\wunder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B7BF2-3BCE-4413-98FD-FA3A8D7B48D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF376A8B-1898-4332-83EB-99060941DFB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="estaciones" sheetId="1" r:id="rId1"/>
-    <sheet name="db" sheetId="4" r:id="rId2"/>
-    <sheet name="apiKeys" sheetId="2" r:id="rId3"/>
-    <sheet name="tamaño_DB" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="db" sheetId="4" r:id="rId3"/>
+    <sheet name="apiKeys" sheetId="2" r:id="rId4"/>
+    <sheet name="tamaño_DB" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="db">db!$A$1:$D$140</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="306">
   <si>
     <t>ISANLORE34</t>
   </si>
@@ -1539,7 +1540,7 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5889,6 +5890,736 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B6631-9B09-4EB2-BE14-CDBD12F18C00}">
+  <dimension ref="A1:A143"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7406A5-A71D-4461-B5BD-63800EDE98EF}">
   <dimension ref="A1:D140"/>
   <sheetViews>
@@ -7869,12 +8600,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C3B681-42F9-41A2-B521-362FB4730680}">
   <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8231,12 +8962,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A905401-12BF-43E6-A189-B8D84824F13C}">
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cambios introducidos luego de realizar el informe
</commit_message>
<xml_diff>
--- a/info_wunder.xlsx
+++ b/info_wunder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\tecnicatura_ia\adscripcion\wunder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\wunder\wunder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65760D56-8412-4910-8AA3-520A5E924440}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6779BFE-ECAE-45E7-9636-BC767F4B20D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2064,10 +2064,10 @@
     <t>3d80ef4863b6460980ef4863b6160932</t>
   </si>
   <si>
-    <t>c7916775bc5d4d0a916775bc5ddd0a65</t>
-  </si>
-  <si>
     <t>e5659d7c49604f37a59d7c4960cf3701</t>
+  </si>
+  <si>
+    <t>2271a1c25c7c4d22b1a1c25c7cfd224e</t>
   </si>
 </sst>
 </file>
@@ -11044,7 +11044,7 @@
   <dimension ref="A1:F245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11083,7 +11083,7 @@
         <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -11119,7 +11119,7 @@
         <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -11397,9 +11397,10 @@
     <hyperlink ref="A5" r:id="rId1" xr:uid="{A461DFE7-4315-4EC7-913E-A3A81FE43FDB}"/>
     <hyperlink ref="A29" r:id="rId2" xr:uid="{34D95853-67BD-41F6-8836-57B01718FB64}"/>
     <hyperlink ref="A8" r:id="rId3" xr:uid="{15CECE15-D41D-47AE-BD2F-A2CCA37B6A26}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{ACE36BD4-B4AA-440E-B97D-3811D4A42A34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>